<commit_message>
Better in narrow bands
</commit_message>
<xml_diff>
--- a/TrialsSummary.xlsx
+++ b/TrialsSummary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Case</t>
   </si>
@@ -39,6 +39,39 @@
   </si>
   <si>
     <t>maxRandomWalks</t>
+  </si>
+  <si>
+    <t>3ASV-easy</t>
+  </si>
+  <si>
+    <t>3ASV-x4</t>
+  </si>
+  <si>
+    <t>7ASV-easy</t>
+  </si>
+  <si>
+    <t>7ASV-x6</t>
+  </si>
+  <si>
+    <t>NOT FOUND SOLUTION</t>
+  </si>
+  <si>
+    <t>7ASV-x4</t>
+  </si>
+  <si>
+    <t>7ASV-x2</t>
+  </si>
+  <si>
+    <t>Ideas:</t>
+  </si>
+  <si>
+    <t>switch to mode 1 after taking a r point in the narrow section</t>
+  </si>
+  <si>
+    <t>Restart search</t>
+  </si>
+  <si>
+    <t>NOT FOUND</t>
   </si>
 </sst>
 </file>
@@ -74,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,13 +390,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -420,7 +459,448 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>200</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1">
+        <v>200</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1">
+        <v>200</v>
+      </c>
+      <c r="C25">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>200</v>
+      </c>
+      <c r="C26">
+        <v>154</v>
+      </c>
+      <c r="D26">
+        <v>278</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
+        <v>200</v>
+      </c>
+      <c r="C27">
+        <v>154</v>
+      </c>
+      <c r="D27">
+        <v>278</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1">
+        <v>200</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>200</v>
+      </c>
+      <c r="C30">
+        <v>140</v>
+      </c>
+      <c r="D30">
+        <v>205</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <v>200</v>
+      </c>
+      <c r="C35">
+        <v>155</v>
+      </c>
+      <c r="D35">
+        <v>215</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="1">
+        <v>200</v>
+      </c>
+      <c r="C36">
+        <v>147</v>
+      </c>
+      <c r="D36">
+        <v>247</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1">
+        <v>200</v>
+      </c>
+      <c r="C37">
+        <v>147</v>
+      </c>
+      <c r="D37">
+        <v>277</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>200</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
+      </c>
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="D41">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>200</v>
+      </c>
+      <c r="C42">
+        <v>161</v>
+      </c>
+      <c r="D42">
+        <v>180</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>